<commit_message>
product image on top, follows on scroll
</commit_message>
<xml_diff>
--- a/static/data/subcategories_complete.xlsx
+++ b/static/data/subcategories_complete.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\web_proyects\imprenta_gallito\static\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA91AB40-3B25-4966-BE14-CAA7B907D85A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC8CCF40-10B7-48D4-8CA8-1CEB05E3DD3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="subcategories_complete" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">subcategories_complete!$A$1:$G$58</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">subcategories_complete!$A$1:$G$56</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -316,18 +316,9 @@
     <t>/media/subcategory_images/stickers/etiquetas-productos.jpg</t>
   </si>
   <si>
-    <t>calcomanias-vehiculos</t>
-  </si>
-  <si>
-    <t>Calcomanías para Vehículos</t>
-  </si>
-  <si>
     <t>Stickers de gran formato para autos</t>
   </si>
   <si>
-    <t>/media/subcategory_images/stickers/calcomanias-vehiculos.jpg</t>
-  </si>
-  <si>
     <t>polos</t>
   </si>
   <si>
@@ -568,24 +559,9 @@
     <t>invitaciones-papeleria</t>
   </si>
   <si>
-    <t>tarjetas-agradecimiento</t>
-  </si>
-  <si>
     <t>Tarjetas de Agradecimiento</t>
   </si>
   <si>
-    <t>Thank you cards personalizadas</t>
-  </si>
-  <si>
-    <t>invitaciones-cumpleanos</t>
-  </si>
-  <si>
-    <t>Invitaciones de Cumpleaños</t>
-  </si>
-  <si>
-    <t>Invitaciones para fiestas infantiles y adultos</t>
-  </si>
-  <si>
     <t>diseno-logo</t>
   </si>
   <si>
@@ -760,9 +736,6 @@
     <t>Invitaciones y anuncios para todo evento</t>
   </si>
   <si>
-    <t>/media/subcategory_images/invitaciones/invitaciones-y-anuncios.jpg</t>
-  </si>
-  <si>
     <t>bebes</t>
   </si>
   <si>
@@ -772,12 +745,6 @@
     <t>Papelería para eventos de bebés</t>
   </si>
   <si>
-    <t>/media/subcategory_images/invitaciones/bebes.jpg</t>
-  </si>
-  <si>
-    <t>/media/subcategory_images/invitaciones/cumpleanos.jpg</t>
-  </si>
-  <si>
     <t>tarjetas-notas</t>
   </si>
   <si>
@@ -787,9 +754,6 @@
     <t>Tarjetas para notas personales</t>
   </si>
   <si>
-    <t>/media/subcategory_images/invitaciones/tarjetas-de-notas.jpg</t>
-  </si>
-  <si>
     <t>articulos-fiesta</t>
   </si>
   <si>
@@ -799,9 +763,6 @@
     <t>Artículos para fiesta y señalización</t>
   </si>
   <si>
-    <t>/media/subcategory_images/invitaciones/articulos-fiestas-y-senalizacion.jpg</t>
-  </si>
-  <si>
     <t>papeleria-personal</t>
   </si>
   <si>
@@ -811,9 +772,6 @@
     <t>Papalería persona</t>
   </si>
   <si>
-    <t>/media/subcategory_images/invitaciones/tarjetas-de-gracias.jpg</t>
-  </si>
-  <si>
     <t>bodas</t>
   </si>
   <si>
@@ -824,6 +782,48 @@
   </si>
   <si>
     <t>/media/subcategory_images/invitaciones_papeleria/papeleria-personal.jpg</t>
+  </si>
+  <si>
+    <t>/media/subcategory_images/invitaciones_papeleria/invitaciones-y-anuncios.jpg</t>
+  </si>
+  <si>
+    <t>/media/subcategory_images/invitaciones_papeleria/bebes.jpg</t>
+  </si>
+  <si>
+    <t>/media/subcategory_images/invitaciones_papeleria/tarjetas-de-notas.jpg</t>
+  </si>
+  <si>
+    <t>/media/subcategory_images/invitaciones_papeleria/articulos-fiestas-y-senalizacion.jpg</t>
+  </si>
+  <si>
+    <t>Bodas</t>
+  </si>
+  <si>
+    <t>tarjetas-de-gracia</t>
+  </si>
+  <si>
+    <t>Tarjetas de agradecimiento</t>
+  </si>
+  <si>
+    <t>/media/subcategory_images/invitaciones_papeleria/tarjetas-de-gracias.jpg</t>
+  </si>
+  <si>
+    <t>cumpleanos</t>
+  </si>
+  <si>
+    <t>Tarjetas de cumpleaños</t>
+  </si>
+  <si>
+    <t>/media/subcategory_images/invitaciones_papeleria/cumpleanos.jpg</t>
+  </si>
+  <si>
+    <t>/media/subcategory_images/stickers/stickers-vehiculos.jpg</t>
+  </si>
+  <si>
+    <t>stickers-vehiculos</t>
+  </si>
+  <si>
+    <t>Stickers para Vehículos</t>
   </si>
 </sst>
 </file>
@@ -1666,8 +1666,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="A58" sqref="A58:A63"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2185,19 +2185,19 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>97</v>
+        <v>265</v>
       </c>
       <c r="B23" t="s">
-        <v>98</v>
+        <v>266</v>
       </c>
       <c r="C23" t="s">
         <v>82</v>
       </c>
       <c r="D23" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E23" t="s">
-        <v>100</v>
+        <v>264</v>
       </c>
       <c r="F23">
         <v>5</v>
@@ -2208,295 +2208,295 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
+        <v>98</v>
+      </c>
+      <c r="B24" t="s">
+        <v>99</v>
+      </c>
+      <c r="C24" t="s">
+        <v>100</v>
+      </c>
+      <c r="D24" t="s">
         <v>101</v>
       </c>
-      <c r="B24" t="s">
+      <c r="E24" t="s">
         <v>102</v>
-      </c>
-      <c r="C24" t="s">
-        <v>103</v>
-      </c>
-      <c r="D24" t="s">
-        <v>104</v>
-      </c>
-      <c r="E24" t="s">
-        <v>105</v>
       </c>
       <c r="F24">
         <v>1</v>
       </c>
       <c r="G24" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
+        <v>104</v>
+      </c>
+      <c r="B25" t="s">
+        <v>105</v>
+      </c>
+      <c r="C25" t="s">
+        <v>100</v>
+      </c>
+      <c r="D25" t="s">
+        <v>106</v>
+      </c>
+      <c r="E25" t="s">
         <v>107</v>
-      </c>
-      <c r="B25" t="s">
-        <v>108</v>
-      </c>
-      <c r="C25" t="s">
-        <v>103</v>
-      </c>
-      <c r="D25" t="s">
-        <v>109</v>
-      </c>
-      <c r="E25" t="s">
-        <v>110</v>
       </c>
       <c r="F25">
         <v>2</v>
       </c>
       <c r="G25" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
+        <v>108</v>
+      </c>
+      <c r="B26" t="s">
+        <v>109</v>
+      </c>
+      <c r="C26" t="s">
+        <v>100</v>
+      </c>
+      <c r="D26" t="s">
+        <v>110</v>
+      </c>
+      <c r="E26" t="s">
         <v>111</v>
-      </c>
-      <c r="B26" t="s">
-        <v>112</v>
-      </c>
-      <c r="C26" t="s">
-        <v>103</v>
-      </c>
-      <c r="D26" t="s">
-        <v>113</v>
-      </c>
-      <c r="E26" t="s">
-        <v>114</v>
       </c>
       <c r="F26">
         <v>3</v>
       </c>
       <c r="G26" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
+        <v>112</v>
+      </c>
+      <c r="B27" t="s">
+        <v>113</v>
+      </c>
+      <c r="C27" t="s">
+        <v>100</v>
+      </c>
+      <c r="D27" t="s">
+        <v>114</v>
+      </c>
+      <c r="E27" t="s">
         <v>115</v>
-      </c>
-      <c r="B27" t="s">
-        <v>116</v>
-      </c>
-      <c r="C27" t="s">
-        <v>103</v>
-      </c>
-      <c r="D27" t="s">
-        <v>117</v>
-      </c>
-      <c r="E27" t="s">
-        <v>118</v>
       </c>
       <c r="F27">
         <v>4</v>
       </c>
       <c r="G27" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
+        <v>116</v>
+      </c>
+      <c r="B28" t="s">
+        <v>117</v>
+      </c>
+      <c r="C28" t="s">
+        <v>118</v>
+      </c>
+      <c r="D28" t="s">
         <v>119</v>
       </c>
-      <c r="B28" t="s">
+      <c r="E28" t="s">
         <v>120</v>
-      </c>
-      <c r="C28" t="s">
-        <v>121</v>
-      </c>
-      <c r="D28" t="s">
-        <v>122</v>
-      </c>
-      <c r="E28" t="s">
-        <v>123</v>
       </c>
       <c r="F28">
         <v>1</v>
       </c>
       <c r="G28" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
+        <v>121</v>
+      </c>
+      <c r="B29" t="s">
+        <v>122</v>
+      </c>
+      <c r="C29" t="s">
+        <v>118</v>
+      </c>
+      <c r="D29" t="s">
+        <v>123</v>
+      </c>
+      <c r="E29" t="s">
         <v>124</v>
-      </c>
-      <c r="B29" t="s">
-        <v>125</v>
-      </c>
-      <c r="C29" t="s">
-        <v>121</v>
-      </c>
-      <c r="D29" t="s">
-        <v>126</v>
-      </c>
-      <c r="E29" t="s">
-        <v>127</v>
       </c>
       <c r="F29">
         <v>2</v>
       </c>
       <c r="G29" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
+        <v>125</v>
+      </c>
+      <c r="B30" t="s">
+        <v>126</v>
+      </c>
+      <c r="C30" t="s">
+        <v>118</v>
+      </c>
+      <c r="D30" t="s">
+        <v>127</v>
+      </c>
+      <c r="E30" t="s">
         <v>128</v>
-      </c>
-      <c r="B30" t="s">
-        <v>129</v>
-      </c>
-      <c r="C30" t="s">
-        <v>121</v>
-      </c>
-      <c r="D30" t="s">
-        <v>130</v>
-      </c>
-      <c r="E30" t="s">
-        <v>131</v>
       </c>
       <c r="F30">
         <v>3</v>
       </c>
       <c r="G30" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
+        <v>129</v>
+      </c>
+      <c r="B31" t="s">
+        <v>130</v>
+      </c>
+      <c r="C31" t="s">
+        <v>118</v>
+      </c>
+      <c r="D31" t="s">
+        <v>131</v>
+      </c>
+      <c r="E31" t="s">
         <v>132</v>
-      </c>
-      <c r="B31" t="s">
-        <v>133</v>
-      </c>
-      <c r="C31" t="s">
-        <v>121</v>
-      </c>
-      <c r="D31" t="s">
-        <v>134</v>
-      </c>
-      <c r="E31" t="s">
-        <v>135</v>
       </c>
       <c r="F31">
         <v>4</v>
       </c>
       <c r="G31" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
+        <v>133</v>
+      </c>
+      <c r="B32" t="s">
+        <v>134</v>
+      </c>
+      <c r="C32" t="s">
+        <v>118</v>
+      </c>
+      <c r="D32" t="s">
+        <v>135</v>
+      </c>
+      <c r="E32" t="s">
         <v>136</v>
-      </c>
-      <c r="B32" t="s">
-        <v>137</v>
-      </c>
-      <c r="C32" t="s">
-        <v>121</v>
-      </c>
-      <c r="D32" t="s">
-        <v>138</v>
-      </c>
-      <c r="E32" t="s">
-        <v>139</v>
       </c>
       <c r="F32">
         <v>5</v>
       </c>
       <c r="G32" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
+        <v>137</v>
+      </c>
+      <c r="B33" t="s">
+        <v>138</v>
+      </c>
+      <c r="C33" t="s">
+        <v>118</v>
+      </c>
+      <c r="D33" t="s">
+        <v>139</v>
+      </c>
+      <c r="E33" t="s">
         <v>140</v>
-      </c>
-      <c r="B33" t="s">
-        <v>141</v>
-      </c>
-      <c r="C33" t="s">
-        <v>121</v>
-      </c>
-      <c r="D33" t="s">
-        <v>142</v>
-      </c>
-      <c r="E33" t="s">
-        <v>143</v>
       </c>
       <c r="F33">
         <v>6</v>
       </c>
       <c r="G33" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
+        <v>141</v>
+      </c>
+      <c r="B34" t="s">
+        <v>142</v>
+      </c>
+      <c r="C34" t="s">
+        <v>118</v>
+      </c>
+      <c r="D34" t="s">
+        <v>143</v>
+      </c>
+      <c r="E34" t="s">
         <v>144</v>
-      </c>
-      <c r="B34" t="s">
-        <v>145</v>
-      </c>
-      <c r="C34" t="s">
-        <v>121</v>
-      </c>
-      <c r="D34" t="s">
-        <v>146</v>
-      </c>
-      <c r="E34" t="s">
-        <v>147</v>
       </c>
       <c r="F34">
         <v>7</v>
       </c>
       <c r="G34" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
+        <v>145</v>
+      </c>
+      <c r="B35" t="s">
+        <v>146</v>
+      </c>
+      <c r="C35" t="s">
+        <v>118</v>
+      </c>
+      <c r="D35" t="s">
+        <v>147</v>
+      </c>
+      <c r="E35" t="s">
         <v>148</v>
-      </c>
-      <c r="B35" t="s">
-        <v>149</v>
-      </c>
-      <c r="C35" t="s">
-        <v>121</v>
-      </c>
-      <c r="D35" t="s">
-        <v>150</v>
-      </c>
-      <c r="E35" t="s">
-        <v>151</v>
       </c>
       <c r="F35">
         <v>8</v>
       </c>
       <c r="G35" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
+        <v>149</v>
+      </c>
+      <c r="B36" t="s">
+        <v>150</v>
+      </c>
+      <c r="C36" t="s">
+        <v>151</v>
+      </c>
+      <c r="D36" t="s">
         <v>152</v>
       </c>
-      <c r="B36" t="s">
+      <c r="E36" t="s">
         <v>153</v>
-      </c>
-      <c r="C36" t="s">
-        <v>154</v>
-      </c>
-      <c r="D36" t="s">
-        <v>155</v>
-      </c>
-      <c r="E36" t="s">
-        <v>156</v>
       </c>
       <c r="F36">
         <v>1</v>
@@ -2507,19 +2507,19 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
+        <v>154</v>
+      </c>
+      <c r="B37" t="s">
+        <v>155</v>
+      </c>
+      <c r="C37" t="s">
+        <v>151</v>
+      </c>
+      <c r="D37" t="s">
+        <v>156</v>
+      </c>
+      <c r="E37" t="s">
         <v>157</v>
-      </c>
-      <c r="B37" t="s">
-        <v>158</v>
-      </c>
-      <c r="C37" t="s">
-        <v>154</v>
-      </c>
-      <c r="D37" t="s">
-        <v>159</v>
-      </c>
-      <c r="E37" t="s">
-        <v>160</v>
       </c>
       <c r="F37">
         <v>2</v>
@@ -2530,19 +2530,19 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B38" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C38" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D38" t="s">
         <v>95</v>
       </c>
       <c r="E38" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="F38">
         <v>3</v>
@@ -2553,19 +2553,19 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
+        <v>161</v>
+      </c>
+      <c r="B39" t="s">
+        <v>162</v>
+      </c>
+      <c r="C39" t="s">
+        <v>151</v>
+      </c>
+      <c r="D39" t="s">
+        <v>163</v>
+      </c>
+      <c r="E39" t="s">
         <v>164</v>
-      </c>
-      <c r="B39" t="s">
-        <v>165</v>
-      </c>
-      <c r="C39" t="s">
-        <v>154</v>
-      </c>
-      <c r="D39" t="s">
-        <v>166</v>
-      </c>
-      <c r="E39" t="s">
-        <v>167</v>
       </c>
       <c r="F39">
         <v>4</v>
@@ -2576,19 +2576,19 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
+        <v>165</v>
+      </c>
+      <c r="B40" t="s">
+        <v>166</v>
+      </c>
+      <c r="C40" t="s">
+        <v>151</v>
+      </c>
+      <c r="D40" t="s">
+        <v>167</v>
+      </c>
+      <c r="E40" t="s">
         <v>168</v>
-      </c>
-      <c r="B40" t="s">
-        <v>169</v>
-      </c>
-      <c r="C40" t="s">
-        <v>154</v>
-      </c>
-      <c r="D40" t="s">
-        <v>170</v>
-      </c>
-      <c r="E40" t="s">
-        <v>171</v>
       </c>
       <c r="F40">
         <v>5</v>
@@ -2599,19 +2599,19 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
+        <v>169</v>
+      </c>
+      <c r="B41" t="s">
+        <v>170</v>
+      </c>
+      <c r="C41" t="s">
+        <v>151</v>
+      </c>
+      <c r="D41" t="s">
+        <v>171</v>
+      </c>
+      <c r="E41" t="s">
         <v>172</v>
-      </c>
-      <c r="B41" t="s">
-        <v>173</v>
-      </c>
-      <c r="C41" t="s">
-        <v>154</v>
-      </c>
-      <c r="D41" t="s">
-        <v>174</v>
-      </c>
-      <c r="E41" t="s">
-        <v>175</v>
       </c>
       <c r="F41">
         <v>6</v>
@@ -2622,19 +2622,19 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
+        <v>173</v>
+      </c>
+      <c r="B42" t="s">
+        <v>174</v>
+      </c>
+      <c r="C42" t="s">
+        <v>151</v>
+      </c>
+      <c r="D42" t="s">
+        <v>175</v>
+      </c>
+      <c r="E42" t="s">
         <v>176</v>
-      </c>
-      <c r="B42" t="s">
-        <v>177</v>
-      </c>
-      <c r="C42" t="s">
-        <v>154</v>
-      </c>
-      <c r="D42" t="s">
-        <v>178</v>
-      </c>
-      <c r="E42" t="s">
-        <v>179</v>
       </c>
       <c r="F42">
         <v>7</v>
@@ -2645,25 +2645,25 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
+        <v>179</v>
+      </c>
+      <c r="B43" t="s">
+        <v>180</v>
+      </c>
+      <c r="C43" t="s">
         <v>181</v>
       </c>
-      <c r="B43" t="s">
+      <c r="D43" t="s">
         <v>182</v>
       </c>
-      <c r="C43" t="s">
-        <v>180</v>
-      </c>
-      <c r="D43" t="s">
+      <c r="E43" t="s">
         <v>183</v>
       </c>
-      <c r="E43" t="s">
-        <v>262</v>
-      </c>
       <c r="F43">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G43" t="s">
-        <v>106</v>
+        <v>26</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.35">
@@ -2674,16 +2674,16 @@
         <v>185</v>
       </c>
       <c r="C44" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D44" t="s">
         <v>186</v>
       </c>
       <c r="E44" t="s">
-        <v>250</v>
+        <v>187</v>
       </c>
       <c r="F44">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G44" t="s">
         <v>26</v>
@@ -2691,13 +2691,13 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B45" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C45" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="D45" t="s">
         <v>190</v>
@@ -2706,7 +2706,7 @@
         <v>191</v>
       </c>
       <c r="F45">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G45" t="s">
         <v>26</v>
@@ -2720,7 +2720,7 @@
         <v>193</v>
       </c>
       <c r="C46" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="D46" t="s">
         <v>194</v>
@@ -2729,7 +2729,7 @@
         <v>195</v>
       </c>
       <c r="F46">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G46" t="s">
         <v>26</v>
@@ -2743,16 +2743,16 @@
         <v>197</v>
       </c>
       <c r="C47" t="s">
-        <v>189</v>
+        <v>198</v>
       </c>
       <c r="D47" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="E47" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="F47">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G47" t="s">
         <v>26</v>
@@ -2760,22 +2760,22 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B48" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C48" t="s">
-        <v>189</v>
+        <v>198</v>
       </c>
       <c r="D48" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="E48" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="F48">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G48" t="s">
         <v>26</v>
@@ -2783,13 +2783,13 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B49" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C49" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="D49" t="s">
         <v>207</v>
@@ -2798,7 +2798,7 @@
         <v>208</v>
       </c>
       <c r="F49">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G49" t="s">
         <v>26</v>
@@ -2812,7 +2812,7 @@
         <v>210</v>
       </c>
       <c r="C50" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="D50" t="s">
         <v>211</v>
@@ -2821,7 +2821,7 @@
         <v>212</v>
       </c>
       <c r="F50">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G50" t="s">
         <v>26</v>
@@ -2835,16 +2835,16 @@
         <v>214</v>
       </c>
       <c r="C51" t="s">
-        <v>206</v>
+        <v>215</v>
       </c>
       <c r="D51" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="E51" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="F51">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G51" t="s">
         <v>26</v>
@@ -2852,22 +2852,22 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B52" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="C52" t="s">
-        <v>206</v>
+        <v>215</v>
       </c>
       <c r="D52" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="E52" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="F52">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G52" t="s">
         <v>26</v>
@@ -2875,13 +2875,13 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B53" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C53" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="D53" t="s">
         <v>224</v>
@@ -2890,7 +2890,7 @@
         <v>225</v>
       </c>
       <c r="F53">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="G53" t="s">
         <v>26</v>
@@ -2904,7 +2904,7 @@
         <v>227</v>
       </c>
       <c r="C54" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="D54" t="s">
         <v>228</v>
@@ -2913,7 +2913,7 @@
         <v>229</v>
       </c>
       <c r="F54">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G54" t="s">
         <v>26</v>
@@ -2927,7 +2927,7 @@
         <v>231</v>
       </c>
       <c r="C55" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="D55" t="s">
         <v>232</v>
@@ -2936,7 +2936,7 @@
         <v>233</v>
       </c>
       <c r="F55">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G55" t="s">
         <v>26</v>
@@ -2950,16 +2950,16 @@
         <v>235</v>
       </c>
       <c r="C56" t="s">
-        <v>223</v>
+        <v>177</v>
       </c>
       <c r="D56" t="s">
         <v>236</v>
       </c>
       <c r="E56" t="s">
-        <v>237</v>
+        <v>253</v>
       </c>
       <c r="F56">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G56" t="s">
         <v>26</v>
@@ -2967,22 +2967,22 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
+        <v>237</v>
+      </c>
+      <c r="B57" t="s">
         <v>238</v>
       </c>
-      <c r="B57" t="s">
+      <c r="C57" t="s">
+        <v>177</v>
+      </c>
+      <c r="D57" t="s">
         <v>239</v>
       </c>
-      <c r="C57" t="s">
-        <v>223</v>
-      </c>
-      <c r="D57" t="s">
-        <v>240</v>
-      </c>
       <c r="E57" t="s">
-        <v>241</v>
+        <v>254</v>
       </c>
       <c r="F57">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="G57" t="s">
         <v>26</v>
@@ -2990,22 +2990,22 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
+        <v>240</v>
+      </c>
+      <c r="B58" t="s">
+        <v>241</v>
+      </c>
+      <c r="C58" t="s">
+        <v>177</v>
+      </c>
+      <c r="D58" t="s">
         <v>242</v>
       </c>
-      <c r="B58" t="s">
-        <v>243</v>
-      </c>
-      <c r="C58" t="s">
-        <v>180</v>
-      </c>
-      <c r="D58" t="s">
-        <v>244</v>
-      </c>
       <c r="E58" t="s">
-        <v>245</v>
+        <v>255</v>
       </c>
       <c r="F58">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G58" t="s">
         <v>26</v>
@@ -3013,22 +3013,22 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="B59" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C59" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="D59" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="E59" t="s">
-        <v>249</v>
+        <v>256</v>
       </c>
       <c r="F59">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G59" t="s">
         <v>26</v>
@@ -3036,22 +3036,22 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="B60" t="s">
+        <v>247</v>
+      </c>
+      <c r="C60" t="s">
+        <v>177</v>
+      </c>
+      <c r="D60" t="s">
+        <v>248</v>
+      </c>
+      <c r="E60" t="s">
         <v>252</v>
       </c>
-      <c r="C60" t="s">
-        <v>180</v>
-      </c>
-      <c r="D60" t="s">
-        <v>253</v>
-      </c>
-      <c r="E60" t="s">
-        <v>254</v>
-      </c>
       <c r="F60">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G60" t="s">
         <v>26</v>
@@ -3059,22 +3059,22 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="B61" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="C61" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="D61" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="E61" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="F61">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="G61" t="s">
         <v>26</v>
@@ -3082,22 +3082,22 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
+        <v>258</v>
+      </c>
+      <c r="B62" t="s">
+        <v>178</v>
+      </c>
+      <c r="C62" t="s">
+        <v>177</v>
+      </c>
+      <c r="D62" t="s">
         <v>259</v>
       </c>
-      <c r="B62" t="s">
+      <c r="E62" t="s">
         <v>260</v>
       </c>
-      <c r="C62" t="s">
-        <v>180</v>
-      </c>
-      <c r="D62" t="s">
-        <v>261</v>
-      </c>
-      <c r="E62" t="s">
-        <v>266</v>
-      </c>
       <c r="F62">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G62" t="s">
         <v>26</v>
@@ -3105,22 +3105,22 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
+        <v>261</v>
+      </c>
+      <c r="B63" t="s">
+        <v>262</v>
+      </c>
+      <c r="C63" t="s">
+        <v>177</v>
+      </c>
+      <c r="D63" t="s">
+        <v>262</v>
+      </c>
+      <c r="E63" t="s">
         <v>263</v>
       </c>
-      <c r="B63" t="s">
-        <v>264</v>
-      </c>
-      <c r="C63" t="s">
-        <v>180</v>
-      </c>
-      <c r="D63" t="s">
-        <v>264</v>
-      </c>
-      <c r="E63" t="s">
-        <v>265</v>
-      </c>
       <c r="F63">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G63" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
pricing actializado para stickers_etiquetas
</commit_message>
<xml_diff>
--- a/static/data/subcategories_complete.xlsx
+++ b/static/data/subcategories_complete.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\web_proyects\imprenta_gallito\static\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC8CCF40-10B7-48D4-8CA8-1CEB05E3DD3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04F6FCE6-6C48-4E49-B962-CB0AA123B3D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="subcategories_complete" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">subcategories_complete!$A$1:$G$56</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">subcategories_complete!$A$1:$G$57</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="266">
   <si>
     <t>subcategory_slug</t>
   </si>
@@ -265,60 +265,15 @@
     <t>/media/subcategory_images/banners/marcos-displays.jpg</t>
   </si>
   <si>
-    <t>stickers-individuales</t>
-  </si>
-  <si>
-    <t>Stickers Individuales</t>
-  </si>
-  <si>
     <t>stickers-etiquetas</t>
   </si>
   <si>
-    <t>Stickers sueltos personalizados</t>
-  </si>
-  <si>
-    <t>/media/subcategory_images/stickers/stickers-individuales.jpg</t>
-  </si>
-  <si>
-    <t>plancha-stickers</t>
-  </si>
-  <si>
-    <t>Plancha de Stickers</t>
-  </si>
-  <si>
-    <t>Stickers en plancha para múltiples unidades</t>
-  </si>
-  <si>
-    <t>/media/subcategory_images/stickers/plancha-stickers.jpg</t>
-  </si>
-  <si>
-    <t>rollo-stickers</t>
-  </si>
-  <si>
-    <t>Rollo de Stickers</t>
-  </si>
-  <si>
-    <t>Stickers en rollo para producción en volumen</t>
-  </si>
-  <si>
-    <t>/media/subcategory_images/stickers/rollo-stickers.jpg</t>
-  </si>
-  <si>
-    <t>etiquetas-productos</t>
-  </si>
-  <si>
     <t>Etiquetas para Productos</t>
   </si>
   <si>
     <t>Etiquetas adhesivas para empaques</t>
   </si>
   <si>
-    <t>/media/subcategory_images/stickers/etiquetas-productos.jpg</t>
-  </si>
-  <si>
-    <t>Stickers de gran formato para autos</t>
-  </si>
-  <si>
     <t>polos</t>
   </si>
   <si>
@@ -817,13 +772,55 @@
     <t>/media/subcategory_images/invitaciones_papeleria/cumpleanos.jpg</t>
   </si>
   <si>
-    <t>/media/subcategory_images/stickers/stickers-vehiculos.jpg</t>
-  </si>
-  <si>
-    <t>stickers-vehiculos</t>
-  </si>
-  <si>
-    <t>Stickers para Vehículos</t>
+    <t>/media/subcategory_images/stickers/stickers.jpg</t>
+  </si>
+  <si>
+    <t>Stickers personalizados</t>
+  </si>
+  <si>
+    <t>stickers</t>
+  </si>
+  <si>
+    <t>Embalaje personalizado</t>
+  </si>
+  <si>
+    <t>/media/subcategory_images/stickers/embalaje-personalizado.jpg</t>
+  </si>
+  <si>
+    <t>etiquetas</t>
+  </si>
+  <si>
+    <t>/media/subcategory_images/stickers/etiquetas.jpg</t>
+  </si>
+  <si>
+    <t>imanes</t>
+  </si>
+  <si>
+    <t>Imanes personalizados</t>
+  </si>
+  <si>
+    <t>/media/subcategory_images/stickers/imanes.jpg</t>
+  </si>
+  <si>
+    <t>pines</t>
+  </si>
+  <si>
+    <t>Pines personalizados</t>
+  </si>
+  <si>
+    <t>/media/subcategory_images/stickers/pines.jpg</t>
+  </si>
+  <si>
+    <t>acrilicos</t>
+  </si>
+  <si>
+    <t>Acrílicos personalizados</t>
+  </si>
+  <si>
+    <t>/media/subcategory_images/stickers/acrilicos.jpg</t>
+  </si>
+  <si>
+    <t>Stickers  personalizados</t>
   </si>
 </sst>
 </file>
@@ -1664,17 +1661,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G63"/>
+  <dimension ref="A1:G64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="21.54296875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="65.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="74.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
@@ -2093,19 +2091,19 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
+        <v>251</v>
+      </c>
+      <c r="B19" t="s">
+        <v>265</v>
+      </c>
+      <c r="C19" t="s">
         <v>80</v>
       </c>
-      <c r="B19" t="s">
-        <v>81</v>
-      </c>
-      <c r="C19" t="s">
-        <v>82</v>
-      </c>
       <c r="D19" t="s">
-        <v>83</v>
+        <v>250</v>
       </c>
       <c r="E19" t="s">
-        <v>84</v>
+        <v>249</v>
       </c>
       <c r="F19">
         <v>1</v>
@@ -2116,22 +2114,22 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>85</v>
+        <v>136</v>
       </c>
       <c r="B20" t="s">
-        <v>86</v>
+        <v>252</v>
       </c>
       <c r="C20" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D20" t="s">
-        <v>87</v>
+        <v>252</v>
       </c>
       <c r="E20" t="s">
-        <v>88</v>
+        <v>253</v>
       </c>
       <c r="F20">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G20" t="s">
         <v>26</v>
@@ -2139,22 +2137,22 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>89</v>
+        <v>254</v>
       </c>
       <c r="B21" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="C21" t="s">
+        <v>80</v>
+      </c>
+      <c r="D21" t="s">
         <v>82</v>
       </c>
-      <c r="D21" t="s">
-        <v>91</v>
-      </c>
       <c r="E21" t="s">
-        <v>92</v>
+        <v>255</v>
       </c>
       <c r="F21">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G21" t="s">
         <v>26</v>
@@ -2162,22 +2160,22 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>93</v>
+        <v>256</v>
       </c>
       <c r="B22" t="s">
-        <v>94</v>
+        <v>257</v>
       </c>
       <c r="C22" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D22" t="s">
-        <v>95</v>
+        <v>257</v>
       </c>
       <c r="E22" t="s">
-        <v>96</v>
+        <v>258</v>
       </c>
       <c r="F22">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G22" t="s">
         <v>26</v>
@@ -2185,22 +2183,22 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="B23" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="C23" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D23" t="s">
-        <v>97</v>
+        <v>260</v>
       </c>
       <c r="E23" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="F23">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G23" t="s">
         <v>26</v>
@@ -2208,321 +2206,321 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>98</v>
+        <v>262</v>
       </c>
       <c r="B24" t="s">
-        <v>99</v>
+        <v>263</v>
       </c>
       <c r="C24" t="s">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="D24" t="s">
-        <v>101</v>
+        <v>263</v>
       </c>
       <c r="E24" t="s">
-        <v>102</v>
+        <v>264</v>
       </c>
       <c r="F24">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G24" t="s">
-        <v>103</v>
+        <v>26</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>104</v>
+        <v>83</v>
       </c>
       <c r="B25" t="s">
-        <v>105</v>
+        <v>84</v>
       </c>
       <c r="C25" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="D25" t="s">
-        <v>106</v>
+        <v>86</v>
       </c>
       <c r="E25" t="s">
-        <v>107</v>
+        <v>87</v>
       </c>
       <c r="F25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G25" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>108</v>
+        <v>89</v>
       </c>
       <c r="B26" t="s">
-        <v>109</v>
+        <v>90</v>
       </c>
       <c r="C26" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="D26" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="E26" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
       <c r="F26">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G26" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>112</v>
+        <v>93</v>
       </c>
       <c r="B27" t="s">
-        <v>113</v>
+        <v>94</v>
       </c>
       <c r="C27" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="D27" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="E27" t="s">
-        <v>115</v>
+        <v>96</v>
       </c>
       <c r="F27">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G27" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>116</v>
+        <v>97</v>
       </c>
       <c r="B28" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="C28" t="s">
-        <v>118</v>
+        <v>85</v>
       </c>
       <c r="D28" t="s">
-        <v>119</v>
+        <v>99</v>
       </c>
       <c r="E28" t="s">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="F28">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G28" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>121</v>
+        <v>101</v>
       </c>
       <c r="B29" t="s">
-        <v>122</v>
+        <v>102</v>
       </c>
       <c r="C29" t="s">
-        <v>118</v>
+        <v>103</v>
       </c>
       <c r="D29" t="s">
-        <v>123</v>
+        <v>104</v>
       </c>
       <c r="E29" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
       <c r="F29">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G29" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>125</v>
+        <v>106</v>
       </c>
       <c r="B30" t="s">
-        <v>126</v>
+        <v>107</v>
       </c>
       <c r="C30" t="s">
-        <v>118</v>
+        <v>103</v>
       </c>
       <c r="D30" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
       <c r="E30" t="s">
-        <v>128</v>
+        <v>109</v>
       </c>
       <c r="F30">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G30" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>129</v>
+        <v>110</v>
       </c>
       <c r="B31" t="s">
-        <v>130</v>
+        <v>111</v>
       </c>
       <c r="C31" t="s">
-        <v>118</v>
+        <v>103</v>
       </c>
       <c r="D31" t="s">
-        <v>131</v>
+        <v>112</v>
       </c>
       <c r="E31" t="s">
-        <v>132</v>
+        <v>113</v>
       </c>
       <c r="F31">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G31" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>133</v>
+        <v>114</v>
       </c>
       <c r="B32" t="s">
-        <v>134</v>
+        <v>115</v>
       </c>
       <c r="C32" t="s">
-        <v>118</v>
+        <v>103</v>
       </c>
       <c r="D32" t="s">
-        <v>135</v>
+        <v>116</v>
       </c>
       <c r="E32" t="s">
-        <v>136</v>
+        <v>117</v>
       </c>
       <c r="F32">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G32" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>137</v>
+        <v>118</v>
       </c>
       <c r="B33" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
       <c r="C33" t="s">
-        <v>118</v>
+        <v>103</v>
       </c>
       <c r="D33" t="s">
-        <v>139</v>
+        <v>120</v>
       </c>
       <c r="E33" t="s">
-        <v>140</v>
+        <v>121</v>
       </c>
       <c r="F33">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G33" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>141</v>
+        <v>122</v>
       </c>
       <c r="B34" t="s">
-        <v>142</v>
+        <v>123</v>
       </c>
       <c r="C34" t="s">
-        <v>118</v>
+        <v>103</v>
       </c>
       <c r="D34" t="s">
-        <v>143</v>
+        <v>124</v>
       </c>
       <c r="E34" t="s">
-        <v>144</v>
+        <v>125</v>
       </c>
       <c r="F34">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G34" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>145</v>
+        <v>126</v>
       </c>
       <c r="B35" t="s">
-        <v>146</v>
+        <v>127</v>
       </c>
       <c r="C35" t="s">
-        <v>118</v>
+        <v>103</v>
       </c>
       <c r="D35" t="s">
-        <v>147</v>
+        <v>128</v>
       </c>
       <c r="E35" t="s">
-        <v>148</v>
+        <v>129</v>
       </c>
       <c r="F35">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G35" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>149</v>
+        <v>130</v>
       </c>
       <c r="B36" t="s">
-        <v>150</v>
+        <v>131</v>
       </c>
       <c r="C36" t="s">
-        <v>151</v>
+        <v>103</v>
       </c>
       <c r="D36" t="s">
-        <v>152</v>
+        <v>132</v>
       </c>
       <c r="E36" t="s">
-        <v>153</v>
+        <v>133</v>
       </c>
       <c r="F36">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="G36" t="s">
-        <v>26</v>
+        <v>88</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>154</v>
+        <v>134</v>
       </c>
       <c r="B37" t="s">
-        <v>155</v>
+        <v>135</v>
       </c>
       <c r="C37" t="s">
-        <v>151</v>
+        <v>136</v>
       </c>
       <c r="D37" t="s">
-        <v>156</v>
+        <v>137</v>
       </c>
       <c r="E37" t="s">
-        <v>157</v>
+        <v>138</v>
       </c>
       <c r="F37">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G37" t="s">
         <v>26</v>
@@ -2530,22 +2528,22 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>158</v>
+        <v>139</v>
       </c>
       <c r="B38" t="s">
-        <v>159</v>
+        <v>140</v>
       </c>
       <c r="C38" t="s">
-        <v>151</v>
+        <v>136</v>
       </c>
       <c r="D38" t="s">
-        <v>95</v>
+        <v>141</v>
       </c>
       <c r="E38" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="F38">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G38" t="s">
         <v>26</v>
@@ -2553,22 +2551,22 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>161</v>
+        <v>143</v>
       </c>
       <c r="B39" t="s">
-        <v>162</v>
+        <v>144</v>
       </c>
       <c r="C39" t="s">
-        <v>151</v>
+        <v>136</v>
       </c>
       <c r="D39" t="s">
-        <v>163</v>
+        <v>82</v>
       </c>
       <c r="E39" t="s">
-        <v>164</v>
+        <v>145</v>
       </c>
       <c r="F39">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G39" t="s">
         <v>26</v>
@@ -2576,22 +2574,22 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>165</v>
+        <v>146</v>
       </c>
       <c r="B40" t="s">
-        <v>166</v>
+        <v>147</v>
       </c>
       <c r="C40" t="s">
-        <v>151</v>
+        <v>136</v>
       </c>
       <c r="D40" t="s">
-        <v>167</v>
+        <v>148</v>
       </c>
       <c r="E40" t="s">
-        <v>168</v>
+        <v>149</v>
       </c>
       <c r="F40">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G40" t="s">
         <v>26</v>
@@ -2599,22 +2597,22 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>169</v>
+        <v>150</v>
       </c>
       <c r="B41" t="s">
-        <v>170</v>
+        <v>151</v>
       </c>
       <c r="C41" t="s">
-        <v>151</v>
+        <v>136</v>
       </c>
       <c r="D41" t="s">
-        <v>171</v>
+        <v>152</v>
       </c>
       <c r="E41" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
       <c r="F41">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G41" t="s">
         <v>26</v>
@@ -2622,22 +2620,22 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>173</v>
+        <v>154</v>
       </c>
       <c r="B42" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="C42" t="s">
-        <v>151</v>
+        <v>136</v>
       </c>
       <c r="D42" t="s">
-        <v>175</v>
+        <v>156</v>
       </c>
       <c r="E42" t="s">
-        <v>176</v>
+        <v>157</v>
       </c>
       <c r="F42">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G42" t="s">
         <v>26</v>
@@ -2645,19 +2643,19 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>179</v>
+        <v>158</v>
       </c>
       <c r="B43" t="s">
-        <v>180</v>
+        <v>159</v>
       </c>
       <c r="C43" t="s">
-        <v>181</v>
+        <v>136</v>
       </c>
       <c r="D43" t="s">
-        <v>182</v>
+        <v>160</v>
       </c>
       <c r="E43" t="s">
-        <v>183</v>
+        <v>161</v>
       </c>
       <c r="F43">
         <v>7</v>
@@ -2668,22 +2666,22 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>184</v>
+        <v>164</v>
       </c>
       <c r="B44" t="s">
-        <v>185</v>
+        <v>165</v>
       </c>
       <c r="C44" t="s">
-        <v>181</v>
+        <v>166</v>
       </c>
       <c r="D44" t="s">
-        <v>186</v>
+        <v>167</v>
       </c>
       <c r="E44" t="s">
-        <v>187</v>
+        <v>168</v>
       </c>
       <c r="F44">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G44" t="s">
         <v>26</v>
@@ -2691,22 +2689,22 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
       <c r="B45" t="s">
-        <v>189</v>
+        <v>170</v>
       </c>
       <c r="C45" t="s">
-        <v>181</v>
+        <v>166</v>
       </c>
       <c r="D45" t="s">
-        <v>190</v>
+        <v>171</v>
       </c>
       <c r="E45" t="s">
-        <v>191</v>
+        <v>172</v>
       </c>
       <c r="F45">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G45" t="s">
         <v>26</v>
@@ -2714,22 +2712,22 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>192</v>
+        <v>173</v>
       </c>
       <c r="B46" t="s">
-        <v>193</v>
+        <v>174</v>
       </c>
       <c r="C46" t="s">
-        <v>181</v>
+        <v>166</v>
       </c>
       <c r="D46" t="s">
-        <v>194</v>
+        <v>175</v>
       </c>
       <c r="E46" t="s">
-        <v>195</v>
+        <v>176</v>
       </c>
       <c r="F46">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G46" t="s">
         <v>26</v>
@@ -2737,22 +2735,22 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>196</v>
+        <v>177</v>
       </c>
       <c r="B47" t="s">
-        <v>197</v>
+        <v>178</v>
       </c>
       <c r="C47" t="s">
-        <v>198</v>
+        <v>166</v>
       </c>
       <c r="D47" t="s">
-        <v>199</v>
+        <v>179</v>
       </c>
       <c r="E47" t="s">
-        <v>200</v>
+        <v>180</v>
       </c>
       <c r="F47">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G47" t="s">
         <v>26</v>
@@ -2760,22 +2758,22 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>201</v>
+        <v>181</v>
       </c>
       <c r="B48" t="s">
-        <v>202</v>
+        <v>182</v>
       </c>
       <c r="C48" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="D48" t="s">
-        <v>203</v>
+        <v>184</v>
       </c>
       <c r="E48" t="s">
-        <v>204</v>
+        <v>185</v>
       </c>
       <c r="F48">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G48" t="s">
         <v>26</v>
@@ -2783,22 +2781,22 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>205</v>
+        <v>186</v>
       </c>
       <c r="B49" t="s">
-        <v>206</v>
+        <v>187</v>
       </c>
       <c r="C49" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="D49" t="s">
-        <v>207</v>
+        <v>188</v>
       </c>
       <c r="E49" t="s">
-        <v>208</v>
+        <v>189</v>
       </c>
       <c r="F49">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G49" t="s">
         <v>26</v>
@@ -2806,22 +2804,22 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>209</v>
+        <v>190</v>
       </c>
       <c r="B50" t="s">
-        <v>210</v>
+        <v>191</v>
       </c>
       <c r="C50" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="D50" t="s">
-        <v>211</v>
+        <v>192</v>
       </c>
       <c r="E50" t="s">
-        <v>212</v>
+        <v>193</v>
       </c>
       <c r="F50">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G50" t="s">
         <v>26</v>
@@ -2829,22 +2827,22 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>213</v>
+        <v>194</v>
       </c>
       <c r="B51" t="s">
-        <v>214</v>
+        <v>195</v>
       </c>
       <c r="C51" t="s">
-        <v>215</v>
+        <v>183</v>
       </c>
       <c r="D51" t="s">
-        <v>216</v>
+        <v>196</v>
       </c>
       <c r="E51" t="s">
-        <v>217</v>
+        <v>197</v>
       </c>
       <c r="F51">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G51" t="s">
         <v>26</v>
@@ -2852,22 +2850,22 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>218</v>
+        <v>198</v>
       </c>
       <c r="B52" t="s">
-        <v>219</v>
+        <v>199</v>
       </c>
       <c r="C52" t="s">
-        <v>215</v>
+        <v>200</v>
       </c>
       <c r="D52" t="s">
-        <v>220</v>
+        <v>201</v>
       </c>
       <c r="E52" t="s">
-        <v>221</v>
+        <v>202</v>
       </c>
       <c r="F52">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G52" t="s">
         <v>26</v>
@@ -2875,22 +2873,22 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>222</v>
+        <v>203</v>
       </c>
       <c r="B53" t="s">
-        <v>223</v>
+        <v>204</v>
       </c>
       <c r="C53" t="s">
-        <v>215</v>
+        <v>200</v>
       </c>
       <c r="D53" t="s">
-        <v>224</v>
+        <v>205</v>
       </c>
       <c r="E53" t="s">
-        <v>225</v>
+        <v>206</v>
       </c>
       <c r="F53">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="G53" t="s">
         <v>26</v>
@@ -2898,22 +2896,22 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>226</v>
+        <v>207</v>
       </c>
       <c r="B54" t="s">
-        <v>227</v>
+        <v>208</v>
       </c>
       <c r="C54" t="s">
-        <v>215</v>
+        <v>200</v>
       </c>
       <c r="D54" t="s">
-        <v>228</v>
+        <v>209</v>
       </c>
       <c r="E54" t="s">
-        <v>229</v>
+        <v>210</v>
       </c>
       <c r="F54">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="G54" t="s">
         <v>26</v>
@@ -2921,22 +2919,22 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>230</v>
+        <v>211</v>
       </c>
       <c r="B55" t="s">
-        <v>231</v>
+        <v>212</v>
       </c>
       <c r="C55" t="s">
-        <v>215</v>
+        <v>200</v>
       </c>
       <c r="D55" t="s">
-        <v>232</v>
+        <v>213</v>
       </c>
       <c r="E55" t="s">
-        <v>233</v>
+        <v>214</v>
       </c>
       <c r="F55">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G55" t="s">
         <v>26</v>
@@ -2944,22 +2942,22 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>234</v>
+        <v>215</v>
       </c>
       <c r="B56" t="s">
-        <v>235</v>
+        <v>216</v>
       </c>
       <c r="C56" t="s">
-        <v>177</v>
+        <v>200</v>
       </c>
       <c r="D56" t="s">
-        <v>236</v>
+        <v>217</v>
       </c>
       <c r="E56" t="s">
-        <v>253</v>
+        <v>218</v>
       </c>
       <c r="F56">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G56" t="s">
         <v>26</v>
@@ -2967,22 +2965,22 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>237</v>
+        <v>219</v>
       </c>
       <c r="B57" t="s">
+        <v>220</v>
+      </c>
+      <c r="C57" t="s">
+        <v>162</v>
+      </c>
+      <c r="D57" t="s">
+        <v>221</v>
+      </c>
+      <c r="E57" t="s">
         <v>238</v>
       </c>
-      <c r="C57" t="s">
-        <v>177</v>
-      </c>
-      <c r="D57" t="s">
-        <v>239</v>
-      </c>
-      <c r="E57" t="s">
-        <v>254</v>
-      </c>
       <c r="F57">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G57" t="s">
         <v>26</v>
@@ -2990,22 +2988,22 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>240</v>
+        <v>222</v>
       </c>
       <c r="B58" t="s">
-        <v>241</v>
+        <v>223</v>
       </c>
       <c r="C58" t="s">
-        <v>177</v>
+        <v>162</v>
       </c>
       <c r="D58" t="s">
-        <v>242</v>
+        <v>224</v>
       </c>
       <c r="E58" t="s">
-        <v>255</v>
+        <v>239</v>
       </c>
       <c r="F58">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G58" t="s">
         <v>26</v>
@@ -3013,22 +3011,22 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>243</v>
+        <v>225</v>
       </c>
       <c r="B59" t="s">
-        <v>244</v>
+        <v>226</v>
       </c>
       <c r="C59" t="s">
-        <v>177</v>
+        <v>162</v>
       </c>
       <c r="D59" t="s">
-        <v>245</v>
+        <v>227</v>
       </c>
       <c r="E59" t="s">
-        <v>256</v>
+        <v>240</v>
       </c>
       <c r="F59">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G59" t="s">
         <v>26</v>
@@ -3036,22 +3034,22 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>246</v>
+        <v>228</v>
       </c>
       <c r="B60" t="s">
-        <v>247</v>
+        <v>229</v>
       </c>
       <c r="C60" t="s">
-        <v>177</v>
+        <v>162</v>
       </c>
       <c r="D60" t="s">
-        <v>248</v>
+        <v>230</v>
       </c>
       <c r="E60" t="s">
-        <v>252</v>
+        <v>241</v>
       </c>
       <c r="F60">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G60" t="s">
         <v>26</v>
@@ -3059,22 +3057,22 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>249</v>
+        <v>231</v>
       </c>
       <c r="B61" t="s">
-        <v>257</v>
+        <v>232</v>
       </c>
       <c r="C61" t="s">
-        <v>177</v>
+        <v>162</v>
       </c>
       <c r="D61" t="s">
-        <v>250</v>
+        <v>233</v>
       </c>
       <c r="E61" t="s">
-        <v>251</v>
+        <v>237</v>
       </c>
       <c r="F61">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="G61" t="s">
         <v>26</v>
@@ -3082,22 +3080,22 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>258</v>
+        <v>234</v>
       </c>
       <c r="B62" t="s">
-        <v>178</v>
+        <v>242</v>
       </c>
       <c r="C62" t="s">
-        <v>177</v>
+        <v>162</v>
       </c>
       <c r="D62" t="s">
-        <v>259</v>
+        <v>235</v>
       </c>
       <c r="E62" t="s">
-        <v>260</v>
+        <v>236</v>
       </c>
       <c r="F62">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="G62" t="s">
         <v>26</v>
@@ -3105,24 +3103,47 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>261</v>
+        <v>243</v>
       </c>
       <c r="B63" t="s">
-        <v>262</v>
+        <v>163</v>
       </c>
       <c r="C63" t="s">
-        <v>177</v>
+        <v>162</v>
       </c>
       <c r="D63" t="s">
-        <v>262</v>
+        <v>244</v>
       </c>
       <c r="E63" t="s">
-        <v>263</v>
+        <v>245</v>
       </c>
       <c r="F63">
+        <v>13</v>
+      </c>
+      <c r="G63" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>246</v>
+      </c>
+      <c r="B64" t="s">
+        <v>247</v>
+      </c>
+      <c r="C64" t="s">
+        <v>162</v>
+      </c>
+      <c r="D64" t="s">
+        <v>247</v>
+      </c>
+      <c r="E64" t="s">
+        <v>248</v>
+      </c>
+      <c r="F64">
         <v>14</v>
       </c>
-      <c r="G63" t="s">
+      <c r="G64" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>

<commit_message>
solucionado selección de templates
</commit_message>
<xml_diff>
--- a/static/data/subcategories_complete.xlsx
+++ b/static/data/subcategories_complete.xlsx
@@ -8,22 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\web_proyects\imprenta_gallito\static\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04F6FCE6-6C48-4E49-B962-CB0AA123B3D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A5DA446-5E89-4569-8A5D-C2EE83E6AF7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20" yWindow="110" windowWidth="34380" windowHeight="13570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="subcategories_complete" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">subcategories_complete!$A$1:$G$57</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">subcategories_complete!$A$1:$G$52</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="310">
   <si>
     <t>subcategory_slug</t>
   </si>
@@ -619,69 +619,9 @@
     <t>/media/subcategory_images/servicios/diseno-publicitario.jpg</t>
   </si>
   <si>
-    <t>calendarios-pared</t>
-  </si>
-  <si>
-    <t>Calendarios de Pared</t>
-  </si>
-  <si>
     <t>calendarios-regalos</t>
   </si>
   <si>
-    <t>Calendarios grandes para colgar</t>
-  </si>
-  <si>
-    <t>/media/subcategory_images/calendarios/calendarios-pared.jpg</t>
-  </si>
-  <si>
-    <t>calendarios-escritorio</t>
-  </si>
-  <si>
-    <t>Calendarios de Escritorio</t>
-  </si>
-  <si>
-    <t>Calendarios compactos para mesa</t>
-  </si>
-  <si>
-    <t>/media/subcategory_images/calendarios/calendarios-escritorio.jpg</t>
-  </si>
-  <si>
-    <t>agendas-personalizadas</t>
-  </si>
-  <si>
-    <t>Agendas Personalizadas</t>
-  </si>
-  <si>
-    <t>Agendas y planners customizados</t>
-  </si>
-  <si>
-    <t>/media/subcategory_images/calendarios/agendas-personalizadas.jpg</t>
-  </si>
-  <si>
-    <t>libretas-cuadernos</t>
-  </si>
-  <si>
-    <t>Libretas y Cuadernos</t>
-  </si>
-  <si>
-    <t>Cuadernos personalizados</t>
-  </si>
-  <si>
-    <t>/media/subcategory_images/calendarios/libretas-cuadernos.jpg</t>
-  </si>
-  <si>
-    <t>regalos-corporativos</t>
-  </si>
-  <si>
-    <t>Regalos Corporativos</t>
-  </si>
-  <si>
-    <t>Sets de regalo para empresas</t>
-  </si>
-  <si>
-    <t>/media/subcategory_images/calendarios/regalos-corporativos.jpg</t>
-  </si>
-  <si>
     <t>invitaciones-anuncios</t>
   </si>
   <si>
@@ -821,6 +761,198 @@
   </si>
   <si>
     <t>Stickers  personalizados</t>
+  </si>
+  <si>
+    <t>albumes-fotos-familia</t>
+  </si>
+  <si>
+    <t>Albumes Fotos Familia</t>
+  </si>
+  <si>
+    <t>Subcategoría de Albumes Fotos Familia</t>
+  </si>
+  <si>
+    <t>/media/subcategory_images/calendarios_regalos/albumes-fotos-familia.jpg</t>
+  </si>
+  <si>
+    <t>almohadas-mascota-nuevo</t>
+  </si>
+  <si>
+    <t>Almohadas Mascota</t>
+  </si>
+  <si>
+    <t>Subcategoría de Almohadas Mascota</t>
+  </si>
+  <si>
+    <t>/media/subcategory_images/calendarios_regalos/almohadas-mascota-nuevo.jpg</t>
+  </si>
+  <si>
+    <t>arte-pared-familia</t>
+  </si>
+  <si>
+    <t>Arte Pared Familia</t>
+  </si>
+  <si>
+    <t>Subcategoría de Arte Pared Familia</t>
+  </si>
+  <si>
+    <t>/media/subcategory_images/calendarios_regalos/arte-pared-familia.jpg</t>
+  </si>
+  <si>
+    <t>Bebidas Termos Familia</t>
+  </si>
+  <si>
+    <t>Subcategoría de Bebidas Termos Familia</t>
+  </si>
+  <si>
+    <t>bolsas-tote-personalizadas</t>
+  </si>
+  <si>
+    <t>Bolsas Tote Personalizadas</t>
+  </si>
+  <si>
+    <t>Subcategoría de Bolsas Tote Personalizadas</t>
+  </si>
+  <si>
+    <t>/media/subcategory_images/calendarios_regalos/bolsas-tote-personalizadas.jpg</t>
+  </si>
+  <si>
+    <t>Calendarios Familia</t>
+  </si>
+  <si>
+    <t>/media/subcategory_images/calendarios_regalos/calendarios-familia.jpg</t>
+  </si>
+  <si>
+    <t>cartas-juego-personalizadas-nuevo</t>
+  </si>
+  <si>
+    <t>Cartas Juego Personalizadas</t>
+  </si>
+  <si>
+    <t>Subcategoría de Cartas Juego Personalizadas</t>
+  </si>
+  <si>
+    <t>/media/subcategory_images/calendarios_regalos/cartas-juego-personalizadas-nuevo.jpg</t>
+  </si>
+  <si>
+    <t>cobijas-mantas-personalizadas</t>
+  </si>
+  <si>
+    <t>Cobijas Mantas Personalizadas</t>
+  </si>
+  <si>
+    <t>Subcategoría de Cobijas Mantas Personalizadas</t>
+  </si>
+  <si>
+    <t>/media/subcategory_images/calendarios_regalos/cobijas-mantas-personalizadas.jpg</t>
+  </si>
+  <si>
+    <t>decoracion-hogar-familia</t>
+  </si>
+  <si>
+    <t>Decoracion Hogar Familia</t>
+  </si>
+  <si>
+    <t>Subcategoría de Decoracion Hogar Familia</t>
+  </si>
+  <si>
+    <t>/media/subcategory_images/calendarios_regalos/decoracion-hogar-familia.jpg</t>
+  </si>
+  <si>
+    <t>impresiones-canvas-nuevo</t>
+  </si>
+  <si>
+    <t>Impresiones Canvas</t>
+  </si>
+  <si>
+    <t>Subcategoría de Impresiones Canvas</t>
+  </si>
+  <si>
+    <t>/media/subcategory_images/calendarios_regalos/impresiones-canvas-nuevo.jpg</t>
+  </si>
+  <si>
+    <t>mousepad-personalizado</t>
+  </si>
+  <si>
+    <t>Mousepad Personalizado</t>
+  </si>
+  <si>
+    <t>Subcategoría de Mousepad Personalizado</t>
+  </si>
+  <si>
+    <t>/media/subcategory_images/calendarios_regalos/mousepad-personalizado.jpg</t>
+  </si>
+  <si>
+    <t>papeleria-personal-familia</t>
+  </si>
+  <si>
+    <t>Papeleria Personal Familia</t>
+  </si>
+  <si>
+    <t>Subcategoría de Papeleria Personal Familia</t>
+  </si>
+  <si>
+    <t>/media/subcategory_images/calendarios_regalos/papeleria-personal-familia.jpg</t>
+  </si>
+  <si>
+    <t>plantilla-coordenadas-clasicas</t>
+  </si>
+  <si>
+    <t>Plantilla Coordenadas Clasicas</t>
+  </si>
+  <si>
+    <t>Subcategoría de Plantilla Coordenadas Clasicas</t>
+  </si>
+  <si>
+    <t>/media/subcategory_images/calendarios_regalos/plantilla-coordenadas-clasicas.jpg</t>
+  </si>
+  <si>
+    <t>plantilla-monograma-flores</t>
+  </si>
+  <si>
+    <t>Plantilla Monograma Flores</t>
+  </si>
+  <si>
+    <t>Subcategoría de Plantilla Monograma Flores</t>
+  </si>
+  <si>
+    <t>/media/subcategory_images/calendarios_regalos/plantilla-monograma-flores.jpg</t>
+  </si>
+  <si>
+    <t>servilletas-foil-nuevo</t>
+  </si>
+  <si>
+    <t>Servilletas Foil</t>
+  </si>
+  <si>
+    <t>Subcategoría de Servilletas Foil</t>
+  </si>
+  <si>
+    <t>/media/subcategory_images/calendarios_regalos/servilletas-foil-nuevo.jpg</t>
+  </si>
+  <si>
+    <t>tarjetas-notas-personalizadas</t>
+  </si>
+  <si>
+    <t>Tarjetas Notas Personalizadas</t>
+  </si>
+  <si>
+    <t>Subcategoría de Tarjetas Notas Personalizadas</t>
+  </si>
+  <si>
+    <t>/media/subcategory_images/calendarios_regalos/tarjetas-notas-personalizadas.jpg</t>
+  </si>
+  <si>
+    <t>/media/subcategory_images/calendarios_regalos/tazas-termos.jpg</t>
+  </si>
+  <si>
+    <t>tazas-termos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subcategoría de Calendarios </t>
+  </si>
+  <si>
+    <t>calendarios-familiares</t>
   </si>
 </sst>
 </file>
@@ -1661,10 +1793,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G64"/>
+  <dimension ref="A1:G75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="A66" sqref="A66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2091,19 +2223,19 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>251</v>
+        <v>231</v>
       </c>
       <c r="B19" t="s">
-        <v>265</v>
+        <v>245</v>
       </c>
       <c r="C19" t="s">
         <v>80</v>
       </c>
       <c r="D19" t="s">
-        <v>250</v>
+        <v>230</v>
       </c>
       <c r="E19" t="s">
-        <v>249</v>
+        <v>229</v>
       </c>
       <c r="F19">
         <v>1</v>
@@ -2117,16 +2249,16 @@
         <v>136</v>
       </c>
       <c r="B20" t="s">
-        <v>252</v>
+        <v>232</v>
       </c>
       <c r="C20" t="s">
         <v>80</v>
       </c>
       <c r="D20" t="s">
-        <v>252</v>
+        <v>232</v>
       </c>
       <c r="E20" t="s">
-        <v>253</v>
+        <v>233</v>
       </c>
       <c r="F20">
         <v>3</v>
@@ -2137,7 +2269,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>254</v>
+        <v>234</v>
       </c>
       <c r="B21" t="s">
         <v>81</v>
@@ -2149,7 +2281,7 @@
         <v>82</v>
       </c>
       <c r="E21" t="s">
-        <v>255</v>
+        <v>235</v>
       </c>
       <c r="F21">
         <v>4</v>
@@ -2160,19 +2292,19 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>256</v>
+        <v>236</v>
       </c>
       <c r="B22" t="s">
-        <v>257</v>
+        <v>237</v>
       </c>
       <c r="C22" t="s">
         <v>80</v>
       </c>
       <c r="D22" t="s">
-        <v>257</v>
+        <v>237</v>
       </c>
       <c r="E22" t="s">
-        <v>258</v>
+        <v>238</v>
       </c>
       <c r="F22">
         <v>5</v>
@@ -2183,19 +2315,19 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>259</v>
+        <v>239</v>
       </c>
       <c r="B23" t="s">
-        <v>260</v>
+        <v>240</v>
       </c>
       <c r="C23" t="s">
         <v>80</v>
       </c>
       <c r="D23" t="s">
-        <v>260</v>
+        <v>240</v>
       </c>
       <c r="E23" t="s">
-        <v>261</v>
+        <v>241</v>
       </c>
       <c r="F23">
         <v>6</v>
@@ -2206,19 +2338,19 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>262</v>
+        <v>242</v>
       </c>
       <c r="B24" t="s">
-        <v>263</v>
+        <v>243</v>
       </c>
       <c r="C24" t="s">
         <v>80</v>
       </c>
       <c r="D24" t="s">
-        <v>263</v>
+        <v>243</v>
       </c>
       <c r="E24" t="s">
-        <v>264</v>
+        <v>244</v>
       </c>
       <c r="F24">
         <v>7</v>
@@ -2850,22 +2982,22 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B52" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C52" t="s">
-        <v>200</v>
+        <v>162</v>
       </c>
       <c r="D52" t="s">
         <v>201</v>
       </c>
       <c r="E52" t="s">
-        <v>202</v>
+        <v>218</v>
       </c>
       <c r="F52">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G52" t="s">
         <v>26</v>
@@ -2873,22 +3005,22 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
+        <v>202</v>
+      </c>
+      <c r="B53" t="s">
         <v>203</v>
       </c>
-      <c r="B53" t="s">
+      <c r="C53" t="s">
+        <v>162</v>
+      </c>
+      <c r="D53" t="s">
         <v>204</v>
       </c>
-      <c r="C53" t="s">
-        <v>200</v>
-      </c>
-      <c r="D53" t="s">
-        <v>205</v>
-      </c>
       <c r="E53" t="s">
-        <v>206</v>
+        <v>219</v>
       </c>
       <c r="F53">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="G53" t="s">
         <v>26</v>
@@ -2896,22 +3028,22 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
+        <v>205</v>
+      </c>
+      <c r="B54" t="s">
+        <v>206</v>
+      </c>
+      <c r="C54" t="s">
+        <v>162</v>
+      </c>
+      <c r="D54" t="s">
         <v>207</v>
       </c>
-      <c r="B54" t="s">
-        <v>208</v>
-      </c>
-      <c r="C54" t="s">
-        <v>200</v>
-      </c>
-      <c r="D54" t="s">
-        <v>209</v>
-      </c>
       <c r="E54" t="s">
-        <v>210</v>
+        <v>220</v>
       </c>
       <c r="F54">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G54" t="s">
         <v>26</v>
@@ -2919,22 +3051,22 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B55" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C55" t="s">
-        <v>200</v>
+        <v>162</v>
       </c>
       <c r="D55" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="E55" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="F55">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="G55" t="s">
         <v>26</v>
@@ -2942,22 +3074,22 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="B56" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="C56" t="s">
-        <v>200</v>
+        <v>162</v>
       </c>
       <c r="D56" t="s">
+        <v>213</v>
+      </c>
+      <c r="E56" t="s">
         <v>217</v>
       </c>
-      <c r="E56" t="s">
-        <v>218</v>
-      </c>
       <c r="F56">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="G56" t="s">
         <v>26</v>
@@ -2965,22 +3097,22 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="B57" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="C57" t="s">
         <v>162</v>
       </c>
       <c r="D57" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="E57" t="s">
-        <v>238</v>
+        <v>216</v>
       </c>
       <c r="F57">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G57" t="s">
         <v>26</v>
@@ -2988,10 +3120,10 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B58" t="s">
-        <v>223</v>
+        <v>163</v>
       </c>
       <c r="C58" t="s">
         <v>162</v>
@@ -3000,10 +3132,10 @@
         <v>224</v>
       </c>
       <c r="E58" t="s">
-        <v>239</v>
+        <v>225</v>
       </c>
       <c r="F58">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="G58" t="s">
         <v>26</v>
@@ -3011,10 +3143,10 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B59" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C59" t="s">
         <v>162</v>
@@ -3023,10 +3155,10 @@
         <v>227</v>
       </c>
       <c r="E59" t="s">
-        <v>240</v>
+        <v>228</v>
       </c>
       <c r="F59">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="G59" t="s">
         <v>26</v>
@@ -3034,22 +3166,22 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>228</v>
+        <v>246</v>
       </c>
       <c r="B60" t="s">
-        <v>229</v>
+        <v>247</v>
       </c>
       <c r="C60" t="s">
-        <v>162</v>
+        <v>198</v>
       </c>
       <c r="D60" t="s">
-        <v>230</v>
+        <v>248</v>
       </c>
       <c r="E60" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="F60">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="G60" t="s">
         <v>26</v>
@@ -3057,22 +3189,22 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>231</v>
+        <v>250</v>
       </c>
       <c r="B61" t="s">
-        <v>232</v>
+        <v>251</v>
       </c>
       <c r="C61" t="s">
-        <v>162</v>
+        <v>198</v>
       </c>
       <c r="D61" t="s">
-        <v>233</v>
+        <v>252</v>
       </c>
       <c r="E61" t="s">
-        <v>237</v>
+        <v>253</v>
       </c>
       <c r="F61">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="G61" t="s">
         <v>26</v>
@@ -3080,22 +3212,22 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>234</v>
+        <v>254</v>
       </c>
       <c r="B62" t="s">
-        <v>242</v>
+        <v>255</v>
       </c>
       <c r="C62" t="s">
-        <v>162</v>
+        <v>198</v>
       </c>
       <c r="D62" t="s">
-        <v>235</v>
+        <v>256</v>
       </c>
       <c r="E62" t="s">
-        <v>236</v>
+        <v>257</v>
       </c>
       <c r="F62">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G62" t="s">
         <v>26</v>
@@ -3103,22 +3235,22 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>243</v>
+        <v>307</v>
       </c>
       <c r="B63" t="s">
-        <v>163</v>
+        <v>258</v>
       </c>
       <c r="C63" t="s">
-        <v>162</v>
+        <v>198</v>
       </c>
       <c r="D63" t="s">
-        <v>244</v>
+        <v>259</v>
       </c>
       <c r="E63" t="s">
-        <v>245</v>
+        <v>306</v>
       </c>
       <c r="F63">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="G63" t="s">
         <v>26</v>
@@ -3126,24 +3258,277 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>246</v>
+        <v>260</v>
       </c>
       <c r="B64" t="s">
-        <v>247</v>
+        <v>261</v>
       </c>
       <c r="C64" t="s">
-        <v>162</v>
+        <v>198</v>
       </c>
       <c r="D64" t="s">
-        <v>247</v>
+        <v>262</v>
       </c>
       <c r="E64" t="s">
-        <v>248</v>
+        <v>263</v>
       </c>
       <c r="F64">
+        <v>5</v>
+      </c>
+      <c r="G64" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>309</v>
+      </c>
+      <c r="B65" t="s">
+        <v>264</v>
+      </c>
+      <c r="C65" t="s">
+        <v>198</v>
+      </c>
+      <c r="D65" t="s">
+        <v>308</v>
+      </c>
+      <c r="E65" t="s">
+        <v>265</v>
+      </c>
+      <c r="F65">
+        <v>6</v>
+      </c>
+      <c r="G65" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>266</v>
+      </c>
+      <c r="B66" t="s">
+        <v>267</v>
+      </c>
+      <c r="C66" t="s">
+        <v>198</v>
+      </c>
+      <c r="D66" t="s">
+        <v>268</v>
+      </c>
+      <c r="E66" t="s">
+        <v>269</v>
+      </c>
+      <c r="F66">
+        <v>7</v>
+      </c>
+      <c r="G66" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>270</v>
+      </c>
+      <c r="B67" t="s">
+        <v>271</v>
+      </c>
+      <c r="C67" t="s">
+        <v>198</v>
+      </c>
+      <c r="D67" t="s">
+        <v>272</v>
+      </c>
+      <c r="E67" t="s">
+        <v>273</v>
+      </c>
+      <c r="F67">
+        <v>8</v>
+      </c>
+      <c r="G67" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>274</v>
+      </c>
+      <c r="B68" t="s">
+        <v>275</v>
+      </c>
+      <c r="C68" t="s">
+        <v>198</v>
+      </c>
+      <c r="D68" t="s">
+        <v>276</v>
+      </c>
+      <c r="E68" t="s">
+        <v>277</v>
+      </c>
+      <c r="F68">
+        <v>9</v>
+      </c>
+      <c r="G68" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>278</v>
+      </c>
+      <c r="B69" t="s">
+        <v>279</v>
+      </c>
+      <c r="C69" t="s">
+        <v>198</v>
+      </c>
+      <c r="D69" t="s">
+        <v>280</v>
+      </c>
+      <c r="E69" t="s">
+        <v>281</v>
+      </c>
+      <c r="F69">
+        <v>10</v>
+      </c>
+      <c r="G69" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>282</v>
+      </c>
+      <c r="B70" t="s">
+        <v>283</v>
+      </c>
+      <c r="C70" t="s">
+        <v>198</v>
+      </c>
+      <c r="D70" t="s">
+        <v>284</v>
+      </c>
+      <c r="E70" t="s">
+        <v>285</v>
+      </c>
+      <c r="F70">
+        <v>11</v>
+      </c>
+      <c r="G70" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>286</v>
+      </c>
+      <c r="B71" t="s">
+        <v>287</v>
+      </c>
+      <c r="C71" t="s">
+        <v>198</v>
+      </c>
+      <c r="D71" t="s">
+        <v>288</v>
+      </c>
+      <c r="E71" t="s">
+        <v>289</v>
+      </c>
+      <c r="F71">
+        <v>12</v>
+      </c>
+      <c r="G71" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
+        <v>290</v>
+      </c>
+      <c r="B72" t="s">
+        <v>291</v>
+      </c>
+      <c r="C72" t="s">
+        <v>198</v>
+      </c>
+      <c r="D72" t="s">
+        <v>292</v>
+      </c>
+      <c r="E72" t="s">
+        <v>293</v>
+      </c>
+      <c r="F72">
+        <v>13</v>
+      </c>
+      <c r="G72" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
+        <v>294</v>
+      </c>
+      <c r="B73" t="s">
+        <v>295</v>
+      </c>
+      <c r="C73" t="s">
+        <v>198</v>
+      </c>
+      <c r="D73" t="s">
+        <v>296</v>
+      </c>
+      <c r="E73" t="s">
+        <v>297</v>
+      </c>
+      <c r="F73">
         <v>14</v>
       </c>
-      <c r="G64" t="s">
+      <c r="G73" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
+        <v>298</v>
+      </c>
+      <c r="B74" t="s">
+        <v>299</v>
+      </c>
+      <c r="C74" t="s">
+        <v>198</v>
+      </c>
+      <c r="D74" t="s">
+        <v>300</v>
+      </c>
+      <c r="E74" t="s">
+        <v>301</v>
+      </c>
+      <c r="F74">
+        <v>15</v>
+      </c>
+      <c r="G74" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
+        <v>302</v>
+      </c>
+      <c r="B75" t="s">
+        <v>303</v>
+      </c>
+      <c r="C75" t="s">
+        <v>198</v>
+      </c>
+      <c r="D75" t="s">
+        <v>304</v>
+      </c>
+      <c r="E75" t="s">
+        <v>305</v>
+      </c>
+      <c r="F75">
+        <v>16</v>
+      </c>
+      <c r="G75" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>